<commit_message>
Height change(7,8,35,36,37,38) - 0.95m
</commit_message>
<xml_diff>
--- a/Gazebo Abu Bhabi inside Lab.xlsx
+++ b/Gazebo Abu Bhabi inside Lab.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>No</t>
   </si>
@@ -67,10 +67,7 @@
     <t>0.383625 m</t>
   </si>
   <si>
-    <t>0.379937 m</t>
-  </si>
-  <si>
-    <t>0.230767 m</t>
+    <t>0.95 m</t>
   </si>
   <si>
     <t>1.42112 m</t>
@@ -149,18 +146,6 @@
   </si>
   <si>
     <t>0.924475 m</t>
-  </si>
-  <si>
-    <t>1.45198 m</t>
-  </si>
-  <si>
-    <t>0.993858 m</t>
-  </si>
-  <si>
-    <t>1.49591 m</t>
-  </si>
-  <si>
-    <t>1.5345 m</t>
   </si>
   <si>
     <t>1.37938 m</t>
@@ -206,7 +191,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -221,6 +206,7 @@
       <color rgb="FF1155CC"/>
       <name val="Inconsolata"/>
     </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -242,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -251,6 +237,9 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -809,7 +798,7 @@
         <f t="shared" si="6"/>
         <v>1.921953517</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -853,8 +842,8 @@
         <f t="shared" si="6"/>
         <v>1.7155615</v>
       </c>
-      <c r="Q9" s="1" t="s">
-        <v>19</v>
+      <c r="Q9" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -898,7 +887,7 @@
         <v>2.267620943</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
@@ -942,7 +931,7 @@
         <v>1.30224119</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
@@ -986,7 +975,7 @@
         <v>2.269555993</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
@@ -1030,7 +1019,7 @@
         <v>2.253699828</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14">
@@ -1074,7 +1063,7 @@
         <v>2.259616219</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15">
@@ -1118,7 +1107,7 @@
         <v>1.335178907</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
@@ -1162,7 +1151,7 @@
         <v>-0.7712297368</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17">
@@ -1206,7 +1195,7 @@
         <v>-2.608895988</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18">
@@ -1250,7 +1239,7 @@
         <v>-0.347679108</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19">
@@ -1294,7 +1283,7 @@
         <v>-1.175395044</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20">
@@ -1338,7 +1327,7 @@
         <v>-2.047245262</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21">
@@ -1382,7 +1371,7 @@
         <v>-3.26215059</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22">
@@ -1426,7 +1415,7 @@
         <v>-2.444117717</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23">
@@ -1470,7 +1459,7 @@
         <v>-1.182128204</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24">
@@ -1514,7 +1503,7 @@
         <v>-2.332927685</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25">
@@ -1558,7 +1547,7 @@
         <v>-0.981290814</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26">
@@ -1602,7 +1591,7 @@
         <v>-2.1392258</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27">
@@ -1646,7 +1635,7 @@
         <v>-3.215256387</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28">
@@ -1690,7 +1679,7 @@
         <v>-0.941649459</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29">
@@ -1734,7 +1723,7 @@
         <v>-2.563152108</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30">
@@ -1778,7 +1767,7 @@
         <v>-2.580290294</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31">
@@ -1822,7 +1811,7 @@
         <v>-0.914653633</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32">
@@ -1866,7 +1855,7 @@
         <v>-2.553179262</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33">
@@ -1910,7 +1899,7 @@
         <v>-1.307476505</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34">
@@ -1954,7 +1943,7 @@
         <v>-2.174431321</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35">
@@ -1998,7 +1987,7 @@
         <v>-3.274154907</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36">
@@ -2041,8 +2030,8 @@
         <f t="shared" si="6"/>
         <v>-1.293981881</v>
       </c>
-      <c r="Q36" s="1" t="s">
-        <v>46</v>
+      <c r="Q36" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="37">
@@ -2085,8 +2074,8 @@
         <f t="shared" si="6"/>
         <v>-2.540626293</v>
       </c>
-      <c r="Q37" s="1" t="s">
-        <v>47</v>
+      <c r="Q37" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="38">
@@ -2129,8 +2118,8 @@
         <f t="shared" si="6"/>
         <v>-0.569203645</v>
       </c>
-      <c r="Q38" s="1" t="s">
-        <v>48</v>
+      <c r="Q38" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="39">
@@ -2173,8 +2162,8 @@
         <f t="shared" si="6"/>
         <v>-1.408322263</v>
       </c>
-      <c r="Q39" s="1" t="s">
-        <v>49</v>
+      <c r="Q39" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="40">
@@ -2218,7 +2207,7 @@
         <v>-2.491814803</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41">
@@ -2262,7 +2251,7 @@
         <v>-0.919118522</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42">
@@ -2306,7 +2295,7 @@
         <v>-2.490034089</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43">
@@ -2350,7 +2339,7 @@
         <v>-0.936044925</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44">
@@ -2394,7 +2383,7 @@
         <v>-2.506045833</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45">
@@ -2438,7 +2427,7 @@
         <v>-0.912146999</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46">
@@ -2482,7 +2471,7 @@
         <v>-2.577737624</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47">
@@ -2526,7 +2515,7 @@
         <v>-0.9719457367</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48">
@@ -2570,7 +2559,7 @@
         <v>-0.5439890205</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49">
@@ -2614,7 +2603,7 @@
         <v>-1.247424627</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50">
@@ -2658,7 +2647,7 @@
         <v>-2.21625484</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51">
@@ -2702,7 +2691,7 @@
         <v>-3.304254236</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52">
@@ -2746,7 +2735,7 @@
         <v>-2.00607577</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Height change(35,38) - 0.5m
</commit_message>
<xml_diff>
--- a/Gazebo Abu Bhabi inside Lab.xlsx
+++ b/Gazebo Abu Bhabi inside Lab.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>No</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>0.924475 m</t>
+  </si>
+  <si>
+    <t>0.5 m</t>
   </si>
   <si>
     <t>1.37938 m</t>
@@ -2031,7 +2034,7 @@
         <v>-1.293981881</v>
       </c>
       <c r="Q36" s="4" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37">
@@ -2163,7 +2166,7 @@
         <v>-1.408322263</v>
       </c>
       <c r="Q39" s="4" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40">
@@ -2207,7 +2210,7 @@
         <v>-2.491814803</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41">
@@ -2251,7 +2254,7 @@
         <v>-0.919118522</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42">
@@ -2295,7 +2298,7 @@
         <v>-2.490034089</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43">
@@ -2339,7 +2342,7 @@
         <v>-0.936044925</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44">
@@ -2383,7 +2386,7 @@
         <v>-2.506045833</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45">
@@ -2427,7 +2430,7 @@
         <v>-0.912146999</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46">
@@ -2471,7 +2474,7 @@
         <v>-2.577737624</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47">
@@ -2515,7 +2518,7 @@
         <v>-0.9719457367</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48">
@@ -2559,7 +2562,7 @@
         <v>-0.5439890205</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49">
@@ -2603,7 +2606,7 @@
         <v>-1.247424627</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50">
@@ -2647,7 +2650,7 @@
         <v>-2.21625484</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51">
@@ -2691,7 +2694,7 @@
         <v>-3.304254236</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52">
@@ -2735,7 +2738,7 @@
         <v>-2.00607577</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>